<commit_message>
Updated summary and program metrics tab to have format and better separated equiv and unequiv
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Metrics" sheetId="1" r:id="rId1"/>
@@ -841,7 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
@@ -950,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -959,7 +959,11 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Update formatting and calculations for freq dist and reach by week tabs
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Metrics" sheetId="1" r:id="rId1"/>
@@ -88,6 +88,291 @@
     <t>Increments of 5</t>
   </si>
   <si>
+    <t>Total (Bravo)</t>
+  </si>
+  <si>
+    <t>Target (Bravo)</t>
+  </si>
+  <si>
+    <t>Total (CNBC)</t>
+  </si>
+  <si>
+    <t>Target (CNBC)</t>
+  </si>
+  <si>
+    <t>Total (E!)</t>
+  </si>
+  <si>
+    <t>Target (E!)</t>
+  </si>
+  <si>
+    <t>Total (Golf Channel)</t>
+  </si>
+  <si>
+    <t>Target (Golf Channel)</t>
+  </si>
+  <si>
+    <t>Total (NBCSN)</t>
+  </si>
+  <si>
+    <t>Target (NBCSN)</t>
+  </si>
+  <si>
+    <t>Total (Syfy)</t>
+  </si>
+  <si>
+    <t>Target (Syfy)</t>
+  </si>
+  <si>
+    <t>Total (USA)</t>
+  </si>
+  <si>
+    <t>Target (USA)</t>
+  </si>
+  <si>
+    <t>Total (NBC)</t>
+  </si>
+  <si>
+    <t>Target (NBC)</t>
+  </si>
+  <si>
+    <t>Total (Esquire)</t>
+  </si>
+  <si>
+    <t>Target (Esquire)</t>
+  </si>
+  <si>
+    <t>reach_pct_target (not unique)</t>
+  </si>
+  <si>
+    <t>Total Target Reach</t>
+  </si>
+  <si>
+    <t>NBC Target Reach</t>
+  </si>
+  <si>
+    <t>Bravo</t>
+  </si>
+  <si>
+    <t>CNBC</t>
+  </si>
+  <si>
+    <t>Chiller</t>
+  </si>
+  <si>
+    <t>E!</t>
+  </si>
+  <si>
+    <t>Esquire</t>
+  </si>
+  <si>
+    <t>Golf Channel</t>
+  </si>
+  <si>
+    <t>NBCSN</t>
+  </si>
+  <si>
+    <t>Syfy</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Total Campaign Target Metrics</t>
+  </si>
+  <si>
+    <t>NOTE: All Unoptimized Campaign metrics in this report are based only on the normalized unoptimized campaign</t>
+  </si>
+  <si>
+    <t>Unoptimized Campaign</t>
+  </si>
+  <si>
+    <t>ATP Optimized Campaign</t>
+  </si>
+  <si>
+    <t>Total Budget</t>
+  </si>
+  <si>
+    <t># of Units</t>
+  </si>
+  <si>
+    <t># of Programs</t>
+  </si>
+  <si>
+    <t># of Networks</t>
+  </si>
+  <si>
+    <t>Total Consumer Target Impressions</t>
+  </si>
+  <si>
+    <t>Consumer Target tCPM($)</t>
+  </si>
+  <si>
+    <t>Consumer Target Reach %</t>
+  </si>
+  <si>
+    <t>Consumer Target TRPs</t>
+  </si>
+  <si>
+    <t>Consumer Target Index (impressions based)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumer Target Frequency </t>
+  </si>
+  <si>
+    <t>Consumer Target Reach # of Households</t>
+  </si>
+  <si>
+    <t>Target Impression Composition by Network</t>
+  </si>
+  <si>
+    <t>NBC</t>
+  </si>
+  <si>
+    <t>NBC Target Impression Composition by ATP Daypart</t>
+  </si>
+  <si>
+    <t>*composition based off total NBC, should add to 100%</t>
+  </si>
+  <si>
+    <t>NBC Morning</t>
+  </si>
+  <si>
+    <t>NBC Daytime</t>
+  </si>
+  <si>
+    <t>NBC Early Fringe</t>
+  </si>
+  <si>
+    <t>NBC Prime</t>
+  </si>
+  <si>
+    <t>NBC Late Night</t>
+  </si>
+  <si>
+    <t>NBC Overnight</t>
+  </si>
+  <si>
+    <t>Average Target Index (impression based) by Network</t>
+  </si>
+  <si>
+    <t>Average Target Index (impression based)  of NBC by ATP Daypart</t>
+  </si>
+  <si>
+    <t>% of Target Reached by Network (not unique)</t>
+  </si>
+  <si>
+    <t>% of Target Reached by NBC by ATP Daypart (not unique)</t>
+  </si>
+  <si>
+    <t>target_reach_pct</t>
+  </si>
+  <si>
+    <t>Target Impressions Compostion by Nested Network/Daypart</t>
+  </si>
+  <si>
+    <t>Unoptimized Campaign: % Share Target Impressions</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Daytime</t>
+  </si>
+  <si>
+    <t>Early Fringe</t>
+  </si>
+  <si>
+    <t>Prime</t>
+  </si>
+  <si>
+    <t>Late Night</t>
+  </si>
+  <si>
+    <t>ATP Campaign: % Share Target Impressions</t>
+  </si>
+  <si>
+    <t>Overnight</t>
+  </si>
+  <si>
+    <t>Average Target Index (impressions based) by Nested Network/Daypart</t>
+  </si>
+  <si>
+    <t>Unoptimized Campaign: Target Index</t>
+  </si>
+  <si>
+    <t>Average Target Index  (impressions based) by Nested Network/Daypart</t>
+  </si>
+  <si>
+    <t>ATP Campaign: Target Index</t>
+  </si>
+  <si>
+    <t>Target Reach  (not unique) by Nested Network/Daypart</t>
+  </si>
+  <si>
+    <t>Unoptimized Campaign: Target Reach</t>
+  </si>
+  <si>
+    <t>Target Reach (not unique) by Nested Network/Daypart</t>
+  </si>
+  <si>
+    <t>ATP Campaign: Target Reach</t>
+  </si>
+  <si>
+    <t>Average Target Frequency by Nested Network/Daypart</t>
+  </si>
+  <si>
+    <t>Unoptimized Campaign: Average Target Frequency</t>
+  </si>
+  <si>
+    <t>ATP Campaign: Average Target Frequency</t>
+  </si>
+  <si>
+    <t>Average Target Frequency</t>
+  </si>
+  <si>
+    <t>Average Target Frequency by NBC by ATP Daypart</t>
+  </si>
+  <si>
+    <t>Below data for ATP Campaign only</t>
+  </si>
+  <si>
+    <t>tCPM</t>
+  </si>
+  <si>
+    <t>Target Reach</t>
+  </si>
+  <si>
+    <t>Ave. Target Frequency</t>
+  </si>
+  <si>
+    <t>channel_code</t>
+  </si>
+  <si>
+    <t>ROVI: Please use the sales dollars in our "As Runs" to calculate tCPM</t>
+  </si>
+  <si>
+    <t>Total (Oxygen)</t>
+  </si>
+  <si>
+    <t>Target (Oxygen)</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>Total (MSNBC)</t>
+  </si>
+  <si>
+    <t>Target (MSNBC)</t>
+  </si>
+  <si>
+    <t>MSNBC</t>
+  </si>
+  <si>
     <t>week</t>
   </si>
   <si>
@@ -103,9 +388,6 @@
     <t>impressions_total</t>
   </si>
   <si>
-    <t>avg_freq_total</t>
-  </si>
-  <si>
     <t>reach_target</t>
   </si>
   <si>
@@ -115,299 +397,17 @@
     <t>impressions_target</t>
   </si>
   <si>
-    <t>avg_freq_target</t>
-  </si>
-  <si>
-    <t>Total (Bravo)</t>
-  </si>
-  <si>
-    <t>Target (Bravo)</t>
-  </si>
-  <si>
-    <t>Total (CNBC)</t>
-  </si>
-  <si>
-    <t>Target (CNBC)</t>
-  </si>
-  <si>
-    <t>Total (E!)</t>
-  </si>
-  <si>
-    <t>Target (E!)</t>
-  </si>
-  <si>
-    <t>Total (Golf Channel)</t>
-  </si>
-  <si>
-    <t>Target (Golf Channel)</t>
-  </si>
-  <si>
-    <t>Total (NBCSN)</t>
-  </si>
-  <si>
-    <t>Target (NBCSN)</t>
-  </si>
-  <si>
-    <t>Total (Syfy)</t>
-  </si>
-  <si>
-    <t>Target (Syfy)</t>
-  </si>
-  <si>
-    <t>Total (USA)</t>
-  </si>
-  <si>
-    <t>Target (USA)</t>
-  </si>
-  <si>
-    <t>Total (NBC)</t>
-  </si>
-  <si>
-    <t>Target (NBC)</t>
-  </si>
-  <si>
-    <t>Total (Esquire)</t>
-  </si>
-  <si>
-    <t>Target (Esquire)</t>
-  </si>
-  <si>
-    <t>reach_pct_target (not unique)</t>
-  </si>
-  <si>
-    <t>Total Target Reach</t>
-  </si>
-  <si>
-    <t>NBC Target Reach</t>
-  </si>
-  <si>
-    <t>Bravo</t>
-  </si>
-  <si>
-    <t>CNBC</t>
-  </si>
-  <si>
-    <t>Chiller</t>
-  </si>
-  <si>
-    <t>E!</t>
-  </si>
-  <si>
-    <t>Esquire</t>
-  </si>
-  <si>
-    <t>Golf Channel</t>
-  </si>
-  <si>
-    <t>NBCSN</t>
-  </si>
-  <si>
-    <t>Syfy</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Total Campaign Target Metrics</t>
-  </si>
-  <si>
-    <t>NOTE: All Unoptimized Campaign metrics in this report are based only on the normalized unoptimized campaign</t>
-  </si>
-  <si>
-    <t>Unoptimized Campaign</t>
-  </si>
-  <si>
-    <t>ATP Optimized Campaign</t>
-  </si>
-  <si>
-    <t>Total Budget</t>
-  </si>
-  <si>
-    <t># of Units</t>
-  </si>
-  <si>
-    <t># of Programs</t>
-  </si>
-  <si>
-    <t># of Networks</t>
-  </si>
-  <si>
-    <t>Total Consumer Target Impressions</t>
-  </si>
-  <si>
-    <t>Consumer Target tCPM($)</t>
-  </si>
-  <si>
-    <t>Consumer Target Reach %</t>
-  </si>
-  <si>
-    <t>Consumer Target TRPs</t>
-  </si>
-  <si>
-    <t>Consumer Target Index (impressions based)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumer Target Frequency </t>
-  </si>
-  <si>
-    <t>Consumer Target Reach # of Households</t>
-  </si>
-  <si>
-    <t>Target Impression Composition by Network</t>
-  </si>
-  <si>
-    <t>NBC</t>
-  </si>
-  <si>
-    <t>NBC Target Impression Composition by ATP Daypart</t>
-  </si>
-  <si>
-    <t>*composition based off total NBC, should add to 100%</t>
-  </si>
-  <si>
-    <t>NBC Morning</t>
-  </si>
-  <si>
-    <t>NBC Daytime</t>
-  </si>
-  <si>
-    <t>NBC Early Fringe</t>
-  </si>
-  <si>
-    <t>NBC Prime</t>
-  </si>
-  <si>
-    <t>NBC Late Night</t>
-  </si>
-  <si>
-    <t>NBC Overnight</t>
-  </si>
-  <si>
-    <t>Average Target Index (impression based) by Network</t>
-  </si>
-  <si>
-    <t>Average Target Index (impression based)  of NBC by ATP Daypart</t>
-  </si>
-  <si>
-    <t>% of Target Reached by Network (not unique)</t>
-  </si>
-  <si>
-    <t>% of Target Reached by NBC by ATP Daypart (not unique)</t>
-  </si>
-  <si>
-    <t>target_reach_pct</t>
-  </si>
-  <si>
-    <t>Target Impressions Compostion by Nested Network/Daypart</t>
-  </si>
-  <si>
-    <t>Unoptimized Campaign: % Share Target Impressions</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Morning</t>
-  </si>
-  <si>
-    <t>Daytime</t>
-  </si>
-  <si>
-    <t>Early Fringe</t>
-  </si>
-  <si>
-    <t>Prime</t>
-  </si>
-  <si>
-    <t>Late Night</t>
-  </si>
-  <si>
-    <t>ATP Campaign: % Share Target Impressions</t>
-  </si>
-  <si>
-    <t>Overnight</t>
-  </si>
-  <si>
-    <t>Average Target Index (impressions based) by Nested Network/Daypart</t>
-  </si>
-  <si>
-    <t>Unoptimized Campaign: Target Index</t>
-  </si>
-  <si>
-    <t>Average Target Index  (impressions based) by Nested Network/Daypart</t>
-  </si>
-  <si>
-    <t>ATP Campaign: Target Index</t>
-  </si>
-  <si>
-    <t>Target Reach  (not unique) by Nested Network/Daypart</t>
-  </si>
-  <si>
-    <t>Unoptimized Campaign: Target Reach</t>
-  </si>
-  <si>
-    <t>Target Reach (not unique) by Nested Network/Daypart</t>
-  </si>
-  <si>
-    <t>ATP Campaign: Target Reach</t>
-  </si>
-  <si>
-    <t>Average Target Frequency by Nested Network/Daypart</t>
-  </si>
-  <si>
-    <t>Unoptimized Campaign: Average Target Frequency</t>
-  </si>
-  <si>
-    <t>ATP Campaign: Average Target Frequency</t>
-  </si>
-  <si>
-    <t>Average Target Frequency</t>
-  </si>
-  <si>
-    <t>Average Target Frequency by NBC by ATP Daypart</t>
-  </si>
-  <si>
-    <t>Below data for ATP Campaign only</t>
-  </si>
-  <si>
-    <t>tCPM</t>
-  </si>
-  <si>
-    <t>Target Reach</t>
-  </si>
-  <si>
-    <t>Ave. Target Frequency</t>
-  </si>
-  <si>
-    <t>channel_code</t>
-  </si>
-  <si>
-    <t>ROVI: Please use the sales dollars in our "As Runs" to calculate tCPM</t>
-  </si>
-  <si>
-    <t>Total (Oxygen)</t>
-  </si>
-  <si>
-    <t>Target (Oxygen)</t>
-  </si>
-  <si>
-    <t>Oxygen</t>
-  </si>
-  <si>
-    <t>Total (MSNBC)</t>
-  </si>
-  <si>
-    <t>Target (MSNBC)</t>
-  </si>
-  <si>
-    <t>MSNBC</t>
+    <t>total_frequency</t>
+  </si>
+  <si>
+    <t>target_frequency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -454,6 +454,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -472,7 +480,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -488,14 +496,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -503,6 +518,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -510,6 +528,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -950,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -976,7 +997,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A3:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -985,22 +1006,23 @@
     <col min="1" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1013,47 +1035,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="12" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
+    <row r="1" spans="1:10">
+      <c r="A1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1084,70 +1109,70 @@
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1180,49 +1205,49 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1251,205 +1276,205 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="B17" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="B33" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1459,118 +1484,118 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="B58" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="B67" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1580,108 +1605,108 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C83" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1716,577 +1741,577 @@
   <sheetData>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1">
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1">
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="1" customFormat="1">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="1" customFormat="1">
       <c r="A36" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="1" customFormat="1">
       <c r="A37" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="1" customFormat="1">
       <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="1" customFormat="1">
       <c r="A45" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:14" s="1" customFormat="1">
       <c r="A49" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1">
       <c r="A50" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="B51" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:14" s="1" customFormat="1">
       <c r="A57" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:14" s="1" customFormat="1">
       <c r="A60" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:14" s="1" customFormat="1">
       <c r="A61" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:14">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="1" customFormat="1">
       <c r="A69" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="1" customFormat="1">
       <c r="A73" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="1" customFormat="1">
       <c r="A74" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="B75" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C75" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D75" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E75" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:14" s="1" customFormat="1">
       <c r="A81" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:14" s="1" customFormat="1">
       <c r="A85" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:14" s="1" customFormat="1">
       <c r="A86" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="3"/>
       <c r="B87" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="N87" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:14">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:14">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:14">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:14" s="1" customFormat="1">
       <c r="A94" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="1" customFormat="1">
       <c r="A97" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="B98" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C98" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2296,214 +2321,214 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="1" customFormat="1">
       <c r="A113" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="B114" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C114" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="122" spans="1:4" s="1" customFormat="1">
       <c r="A122" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B123" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C123" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D123" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="D124" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="D125" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="D126" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="D127" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="D128" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="D129" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="D130" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="D131" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="D132" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="D133" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="D134" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="D135" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="D136" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="D137" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="D138" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="D139" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="D140" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Format and separate equiv and unequiv for network reach by week tab
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Metrics" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="131">
   <si>
     <t>Campaign Summary</t>
   </si>
@@ -401,6 +401,24 @@
   </si>
   <si>
     <t>target_frequency</t>
+  </si>
+  <si>
+    <t>Total (Sprout)</t>
+  </si>
+  <si>
+    <t>Target (Sprout)</t>
+  </si>
+  <si>
+    <t>Total (Telemundo)</t>
+  </si>
+  <si>
+    <t>Target (Telemundo)</t>
+  </si>
+  <si>
+    <t>Sprout</t>
+  </si>
+  <si>
+    <t>Telemundo</t>
   </si>
 </sst>
 </file>
@@ -480,8 +498,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -510,7 +536,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -521,6 +547,10 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -531,6 +561,10 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1033,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1045,34 +1079,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1089,90 +1135,104 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A3:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="27" width="19.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
-      <c r="A1" s="1" t="s">
+    <row r="3" spans="1:29">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1188,11 +1248,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A3:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1201,57 +1259,65 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="16" width="25.6640625" customWidth="1"/>
+    <col min="17" max="18" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="3" spans="1:18" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Format and better separate equiv and unequiv for powerpoint tab
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="-1340" yWindow="-18820" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Program Metrics" sheetId="2" r:id="rId2"/>
-    <sheet name="Frequency Distribution" sheetId="3" r:id="rId3"/>
-    <sheet name="Reach by Week" sheetId="4" r:id="rId4"/>
-    <sheet name="Freq Distribution by Net" sheetId="5" r:id="rId5"/>
-    <sheet name="Network Reach by Week" sheetId="6" r:id="rId6"/>
-    <sheet name="Powerpoint Data" sheetId="7" r:id="rId7"/>
-    <sheet name="Appendix" sheetId="8" r:id="rId8"/>
+    <sheet name="Network Daypart" sheetId="9" r:id="rId3"/>
+    <sheet name="Frequency Distribution" sheetId="3" r:id="rId4"/>
+    <sheet name="Reach by Week" sheetId="4" r:id="rId5"/>
+    <sheet name="Freq Distribution by Net" sheetId="5" r:id="rId6"/>
+    <sheet name="Network Reach by Week" sheetId="6" r:id="rId7"/>
+    <sheet name="Powerpoint Data" sheetId="7" r:id="rId8"/>
+    <sheet name="Appendix" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="131">
   <si>
     <t>Campaign Summary</t>
   </si>
@@ -425,7 +426,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,6 +491,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -498,45 +516,53 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="30" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="29" applyFont="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="29" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
+    <cellStyle name="Comma" xfId="29" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -566,6 +592,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1031,6 +1058,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" s="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1065,7 +1111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1133,7 +1179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AC3"/>
   <sheetViews>
@@ -1246,11 +1292,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1326,13 +1372,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C89"/>
+  <dimension ref="A2:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1428,352 +1472,448 @@
       <c r="A18" t="s">
         <v>41</v>
       </c>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>42</v>
       </c>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
+      <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>45</v>
       </c>
+      <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>114</v>
       </c>
+      <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>66</v>
       </c>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>47</v>
       </c>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>111</v>
       </c>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" s="5" customFormat="1"/>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="B33" t="s">
+    <row r="35" spans="1:3">
+      <c r="B35" t="s">
         <v>52</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>71</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>72</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>73</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="B42" t="s">
+    <row r="44" spans="1:3">
+      <c r="B44" t="s">
         <v>52</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>42</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C45" s="8"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>43</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C47" s="8"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>45</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>46</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>114</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>66</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>47</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>111</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" s="5" customFormat="1">
+      <c r="A57" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1" t="s">
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:3" s="5" customFormat="1">
+      <c r="A58" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="1:3" s="5" customFormat="1">
+      <c r="A59" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="9"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="B58" t="s">
+    <row r="62" spans="1:3">
+      <c r="B62" t="s">
         <v>52</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C62" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>73</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C63" s="8"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>74</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="8"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="B67" t="s">
-        <v>52</v>
-      </c>
-      <c r="C67" t="s">
-        <v>53</v>
-      </c>
+      <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="8"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>41</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C68" s="8"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>42</v>
+      <c r="A70" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>43</v>
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>44</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C72" s="7"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>45</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C73" s="7"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>46</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C74" s="7"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>114</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C75" s="7"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>66</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C76" s="7"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>47</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C77" s="7"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>111</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C78" s="7"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>48</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C79" s="7"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>49</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C80" s="7"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>47</v>
+      </c>
+      <c r="C81" s="7"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="A82" t="s">
+        <v>111</v>
+      </c>
+      <c r="C82" s="7"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" t="s">
-        <v>52</v>
-      </c>
-      <c r="C83" t="s">
-        <v>53</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C83" s="7"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>69</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C84" s="7"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>70</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C85" s="7"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>72</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C86" s="7"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>73</v>
+      <c r="A88" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" t="s">
+        <v>52</v>
+      </c>
+      <c r="C89" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>69</v>
+      </c>
+      <c r="C90" s="7"/>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>70</v>
+      </c>
+      <c r="C91" s="7"/>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>73</v>
+      </c>
+      <c r="C94" s="7"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
         <v>74</v>
       </c>
+      <c r="C95" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1786,7 +1926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N141"/>
   <sheetViews>

</xml_diff>

<commit_message>
Format and better separate equiv and unequiv for appendix tab
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-1340" yWindow="-18820" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Metrics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="131">
   <si>
     <t>Campaign Summary</t>
   </si>
@@ -516,7 +516,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -548,8 +548,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -560,8 +562,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="30" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="29" applyFont="1"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="29" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="30" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="29" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Comma" xfId="29" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -577,6 +583,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -591,6 +598,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
@@ -1376,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1928,11 +1936,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N141"/>
+  <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1940,22 +1946,25 @@
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" customWidth="1"/>
-    <col min="15" max="18" width="37" customWidth="1"/>
+    <col min="5" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" customWidth="1"/>
+    <col min="17" max="20" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="1" spans="1:16">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1">
+    <row r="4" spans="1:16" s="1" customFormat="1">
       <c r="B4" s="1" t="s">
         <v>66</v>
       </c>
@@ -1969,47 +1978,71 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" s="1" customFormat="1">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1">
+    <row r="15" spans="1:16" s="1" customFormat="1">
       <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2047,55 +2080,183 @@
         <v>114</v>
       </c>
       <c r="N15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" s="1" customFormat="1">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+    </row>
+    <row r="22" spans="1:16" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="1" customFormat="1">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+    </row>
+    <row r="25" spans="1:16" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="1" customFormat="1">
+    <row r="26" spans="1:16" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1">
+    <row r="27" spans="1:16" s="1" customFormat="1">
       <c r="B27" s="1" t="s">
         <v>66</v>
       </c>
@@ -2109,47 +2270,71 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" s="1" customFormat="1">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:16" s="1" customFormat="1">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" s="1" customFormat="1">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="36" spans="1:16" s="1" customFormat="1">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="1" customFormat="1">
+    <row r="37" spans="1:16" s="1" customFormat="1">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="1" customFormat="1">
+    <row r="38" spans="1:16" s="1" customFormat="1">
       <c r="B38" s="1" t="s">
         <v>41</v>
       </c>
@@ -2187,55 +2372,166 @@
         <v>114</v>
       </c>
       <c r="N38" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P38" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" s="1" customFormat="1">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+    </row>
+    <row r="45" spans="1:16" s="1" customFormat="1">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" s="1" customFormat="1">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+    </row>
+    <row r="49" spans="1:16" s="1" customFormat="1">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="1" customFormat="1">
+    <row r="50" spans="1:16" s="1" customFormat="1">
       <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:16">
       <c r="B51" t="s">
         <v>66</v>
       </c>
@@ -2249,47 +2545,71 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:16">
       <c r="A52" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" s="1" customFormat="1">
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:16" s="1" customFormat="1">
       <c r="A57" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" s="1" customFormat="1">
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+    </row>
+    <row r="60" spans="1:16" s="1" customFormat="1">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:14" s="1" customFormat="1">
+    <row r="61" spans="1:16" s="1" customFormat="1">
       <c r="A61" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:16">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
         <v>41</v>
@@ -2327,56 +2647,167 @@
       <c r="M62" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N62" s="3" t="s">
+      <c r="N62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P62" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:16">
       <c r="A63" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+      <c r="P63" s="12"/>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+      <c r="P65" s="12"/>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12"/>
+      <c r="P66" s="12"/>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12"/>
+      <c r="P67" s="12"/>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" s="1" customFormat="1">
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="12"/>
+      <c r="P68" s="12"/>
+    </row>
+    <row r="69" spans="1:16" s="1" customFormat="1">
       <c r="A69" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" s="1" customFormat="1">
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+    </row>
+    <row r="73" spans="1:16" s="1" customFormat="1">
       <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="1" customFormat="1">
+    <row r="74" spans="1:16" s="1" customFormat="1">
       <c r="A74" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:16">
       <c r="B75" t="s">
         <v>66</v>
       </c>
@@ -2390,47 +2821,71 @@
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:16">
       <c r="A76" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" s="1" customFormat="1">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+    </row>
+    <row r="81" spans="1:16" s="1" customFormat="1">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" s="1" customFormat="1">
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+    </row>
+    <row r="85" spans="1:16" s="1" customFormat="1">
       <c r="A85" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:14" s="1" customFormat="1">
+    <row r="86" spans="1:16" s="1" customFormat="1">
       <c r="A86" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:16">
       <c r="A87" s="3"/>
       <c r="B87" s="3" t="s">
         <v>41</v>
@@ -2468,44 +2923,155 @@
       <c r="M87" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N87" s="3" t="s">
+      <c r="N87" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P87" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:16">
       <c r="A88" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="8"/>
+      <c r="N88" s="8"/>
+      <c r="O88" s="8"/>
+      <c r="P88" s="8"/>
+    </row>
+    <row r="89" spans="1:16">
       <c r="A89" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="8"/>
+      <c r="N89" s="8"/>
+      <c r="O89" s="8"/>
+      <c r="P89" s="8"/>
+    </row>
+    <row r="90" spans="1:16">
       <c r="A90" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="8"/>
+      <c r="N90" s="8"/>
+      <c r="O90" s="8"/>
+      <c r="P90" s="8"/>
+    </row>
+    <row r="91" spans="1:16">
       <c r="A91" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="92" spans="1:14">
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
+      <c r="J91" s="8"/>
+      <c r="K91" s="8"/>
+      <c r="L91" s="8"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="8"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="8"/>
+    </row>
+    <row r="92" spans="1:16">
       <c r="A92" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="93" spans="1:14">
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="8"/>
+      <c r="K92" s="8"/>
+      <c r="L92" s="8"/>
+      <c r="M92" s="8"/>
+      <c r="N92" s="8"/>
+      <c r="O92" s="8"/>
+      <c r="P92" s="8"/>
+    </row>
+    <row r="93" spans="1:16">
       <c r="A93" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" s="1" customFormat="1">
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
+      <c r="L93" s="8"/>
+      <c r="M93" s="8"/>
+      <c r="N93" s="8"/>
+      <c r="O93" s="8"/>
+      <c r="P93" s="8"/>
+    </row>
+    <row r="94" spans="1:16" s="1" customFormat="1">
       <c r="A94" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="11"/>
+      <c r="L94" s="11"/>
+      <c r="M94" s="11"/>
+      <c r="N94" s="11"/>
+      <c r="O94" s="11"/>
+      <c r="P94" s="11"/>
     </row>
     <row r="97" spans="1:3" s="1" customFormat="1">
       <c r="A97" s="1" t="s">
@@ -2524,216 +3090,335 @@
       <c r="A99" t="s">
         <v>2</v>
       </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>41</v>
       </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>42</v>
       </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>43</v>
       </c>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>44</v>
       </c>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>45</v>
       </c>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>46</v>
       </c>
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>66</v>
       </c>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>47</v>
       </c>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>111</v>
       </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>48</v>
       </c>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>49</v>
       </c>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" s="1" customFormat="1">
-      <c r="A113" s="1" t="s">
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>129</v>
+      </c>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>130</v>
+      </c>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+    </row>
+    <row r="115" spans="1:4" s="1" customFormat="1">
+      <c r="A115" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
-      <c r="B114" t="s">
+    <row r="116" spans="1:4">
+      <c r="B116" t="s">
         <v>52</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C116" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>85</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>86</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>87</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
+        <v>86</v>
+      </c>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>87</v>
+      </c>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" s="1" customFormat="1">
-      <c r="A122" s="1" t="s">
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+    </row>
+    <row r="124" spans="1:4" s="1" customFormat="1">
+      <c r="A124" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
-      <c r="A123" t="s">
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
         <v>104</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B125" t="s">
         <v>105</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C125" t="s">
         <v>106</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D125" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="D124" t="s">
+    <row r="126" spans="1:4">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="8"/>
+      <c r="D126" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
-      <c r="D125" t="s">
+    <row r="127" spans="1:4">
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8"/>
+      <c r="D127" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
-      <c r="D126" t="s">
+    <row r="128" spans="1:4">
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="8"/>
+      <c r="D128" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
-      <c r="D127" t="s">
+    <row r="129" spans="1:4">
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="8"/>
+      <c r="D129" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
-      <c r="D128" t="s">
+    <row r="130" spans="1:4">
+      <c r="A130" s="8"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="8"/>
+      <c r="D130" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="D129" t="s">
+    <row r="131" spans="1:4">
+      <c r="A131" s="8"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="8"/>
+      <c r="D131" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="D130" t="s">
+    <row r="132" spans="1:4">
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+      <c r="D132" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
-      <c r="D131" t="s">
+    <row r="133" spans="1:4">
+      <c r="A133" s="8"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="8"/>
+      <c r="D133" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
-      <c r="D132" t="s">
+    <row r="134" spans="1:4">
+      <c r="A134" s="8"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="8"/>
+      <c r="D134" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
-      <c r="D133" t="s">
+    <row r="135" spans="1:4">
+      <c r="A135" s="8"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="8"/>
+      <c r="D135" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
-      <c r="D134" t="s">
+    <row r="136" spans="1:4">
+      <c r="A136" s="8"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="8"/>
+      <c r="D136" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
-      <c r="D135" t="s">
+    <row r="137" spans="1:4">
+      <c r="A137" s="8"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="8"/>
+      <c r="D137" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="8"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="8"/>
+      <c r="D138" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="8"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="8"/>
+      <c r="D139" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="D136" t="s">
+    <row r="140" spans="1:4">
+      <c r="A140" s="8"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="8"/>
+      <c r="D140" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
-      <c r="D137" t="s">
+    <row r="141" spans="1:4">
+      <c r="A141" s="8"/>
+      <c r="B141" s="8"/>
+      <c r="C141" s="8"/>
+      <c r="D141" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
-      <c r="D138" t="s">
+    <row r="142" spans="1:4">
+      <c r="A142" s="8"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+      <c r="D142" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
-      <c r="D139" t="s">
+    <row r="143" spans="1:4">
+      <c r="A143" s="8"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
+      <c r="D143" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
-      <c r="D140" t="s">
+    <row r="144" spans="1:4">
+      <c r="A144" s="8"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="8"/>
+      <c r="D144" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="2" t="s">
+    <row r="145" spans="1:1">
+      <c r="A145" s="2" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit to have networks in alphabetical order in appropriate tabs
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -516,7 +516,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -548,6 +548,56 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -567,7 +617,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="83">
     <cellStyle name="Comma" xfId="29" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -584,6 +634,31 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -599,6 +674,31 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
@@ -1123,9 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1195,9 +1293,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="27" width="19.6640625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="25" width="19.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="19.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:29">
@@ -1229,64 +1328,64 @@
         <v>25</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="V3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1312,8 +1411,11 @@
     <col min="2" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="16" width="25.6640625" customWidth="1"/>
-    <col min="17" max="18" width="25.1640625" customWidth="1"/>
+    <col min="6" max="14" width="25.6640625" customWidth="1"/>
+    <col min="15" max="15" width="25.1640625" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" customWidth="1"/>
+    <col min="17" max="17" width="25.1640625" customWidth="1"/>
+    <col min="18" max="18" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:18" s="1" customFormat="1">
@@ -1357,16 +1459,16 @@
         <v>111</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1538,25 +1640,25 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="C31" s="7"/>
     </row>
@@ -1695,27 +1797,27 @@
       </c>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" s="5" customFormat="1">
       <c r="A56" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="8"/>
-    </row>
-    <row r="57" spans="1:3" s="5" customFormat="1">
-      <c r="A57" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57" s="9"/>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1">
       <c r="A58" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1">
       <c r="A59" s="6" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="C59" s="9"/>
     </row>
@@ -1849,25 +1951,25 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="C83" s="7"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C84" s="7"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C85" s="7"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="C86" s="7"/>
     </row>
@@ -1936,7 +2038,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P145"/>
+  <dimension ref="A1:Q145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1951,20 +2053,20 @@
     <col min="17" max="20" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1">
+    <row r="4" spans="1:17" s="1" customFormat="1">
       <c r="B4" s="1" t="s">
         <v>66</v>
       </c>
@@ -1978,7 +2080,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -1987,7 +2089,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -1996,7 +2098,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -2005,7 +2107,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2014,7 +2116,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -2023,7 +2125,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1">
+    <row r="10" spans="1:17" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -2032,64 +2134,66 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:17">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="N15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -2315,7 +2419,7 @@
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1">
+    <row r="33" spans="1:17" s="1" customFormat="1">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -2324,64 +2428,66 @@
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="36" spans="1:16" s="1" customFormat="1">
+    <row r="36" spans="1:17" s="1" customFormat="1">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="1" customFormat="1">
+    <row r="37" spans="1:17" s="1" customFormat="1">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1">
-      <c r="B38" s="1" t="s">
+    <row r="38" spans="1:17">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M38" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="N38" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O38" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="3"/>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -2401,7 +2507,7 @@
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -2421,7 +2527,7 @@
       <c r="O40" s="8"/>
       <c r="P40" s="8"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2441,7 +2547,7 @@
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -2461,7 +2567,7 @@
       <c r="O42" s="8"/>
       <c r="P42" s="8"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -2481,7 +2587,7 @@
       <c r="O43" s="8"/>
       <c r="P43" s="8"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2501,7 +2607,7 @@
       <c r="O44" s="8"/>
       <c r="P44" s="8"/>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1">
+    <row r="45" spans="1:17" s="1" customFormat="1">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
@@ -2521,17 +2627,17 @@
       <c r="O45" s="11"/>
       <c r="P45" s="11"/>
     </row>
-    <row r="49" spans="1:16" s="1" customFormat="1">
+    <row r="49" spans="1:17" s="1" customFormat="1">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="1" customFormat="1">
+    <row r="50" spans="1:17" s="1" customFormat="1">
       <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:17">
       <c r="B51" t="s">
         <v>66</v>
       </c>
@@ -2545,7 +2651,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -2554,7 +2660,7 @@
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>84</v>
       </c>
@@ -2563,7 +2669,7 @@
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -2572,7 +2678,7 @@
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -2581,7 +2687,7 @@
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -2590,7 +2696,7 @@
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1">
+    <row r="57" spans="1:17" s="1" customFormat="1">
       <c r="A57" s="1" t="s">
         <v>82</v>
       </c>
@@ -2599,17 +2705,17 @@
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
     </row>
-    <row r="60" spans="1:16" s="1" customFormat="1">
+    <row r="60" spans="1:17" s="1" customFormat="1">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="1" customFormat="1">
+    <row r="61" spans="1:17" s="1" customFormat="1">
       <c r="A61" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:17">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
         <v>41</v>
@@ -2630,34 +2736,35 @@
         <v>46</v>
       </c>
       <c r="H62" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I62" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="J62" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="K62" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K62" s="3" t="s">
+      <c r="L62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M62" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L62" s="3" t="s">
+      <c r="N62" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O62" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M62" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="N62" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P62" s="3" t="s">
+      <c r="P62" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="Q62" s="3"/>
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>83</v>
       </c>
@@ -2677,7 +2784,7 @@
       <c r="O63" s="12"/>
       <c r="P63" s="12"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -2866,7 +2973,7 @@
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:16" s="1" customFormat="1">
+    <row r="81" spans="1:17" s="1" customFormat="1">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
@@ -2875,17 +2982,17 @@
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
     </row>
-    <row r="85" spans="1:16" s="1" customFormat="1">
+    <row r="85" spans="1:17" s="1" customFormat="1">
       <c r="A85" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="1" customFormat="1">
+    <row r="86" spans="1:17" s="1" customFormat="1">
       <c r="A86" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:17">
       <c r="A87" s="3"/>
       <c r="B87" s="3" t="s">
         <v>41</v>
@@ -2906,34 +3013,35 @@
         <v>46</v>
       </c>
       <c r="H87" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I87" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I87" s="3" t="s">
+      <c r="J87" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J87" s="1" t="s">
+      <c r="K87" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K87" s="3" t="s">
+      <c r="L87" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M87" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L87" s="3" t="s">
+      <c r="N87" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O87" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M87" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="N87" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O87" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P87" s="3" t="s">
+      <c r="P87" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="88" spans="1:16">
+      <c r="Q87" s="3"/>
+    </row>
+    <row r="88" spans="1:17">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -2953,7 +3061,7 @@
       <c r="O88" s="8"/>
       <c r="P88" s="8"/>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:17">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -2973,7 +3081,7 @@
       <c r="O89" s="8"/>
       <c r="P89" s="8"/>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:17">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -2993,7 +3101,7 @@
       <c r="O90" s="8"/>
       <c r="P90" s="8"/>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:17">
       <c r="A91" t="s">
         <v>86</v>
       </c>
@@ -3013,7 +3121,7 @@
       <c r="O91" s="8"/>
       <c r="P91" s="8"/>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:17">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -3033,7 +3141,7 @@
       <c r="O92" s="8"/>
       <c r="P92" s="8"/>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:17">
       <c r="A93" t="s">
         <v>89</v>
       </c>
@@ -3053,7 +3161,7 @@
       <c r="O93" s="8"/>
       <c r="P93" s="8"/>
     </row>
-    <row r="94" spans="1:16" s="1" customFormat="1">
+    <row r="94" spans="1:17" s="1" customFormat="1">
       <c r="A94" s="1" t="s">
         <v>82</v>
       </c>
@@ -3137,56 +3245,56 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
@@ -3318,7 +3426,7 @@
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
       <c r="D132" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3326,7 +3434,7 @@
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
       <c r="D133" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3334,7 +3442,7 @@
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
       <c r="D134" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3342,7 +3450,7 @@
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
       <c r="D135" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3350,7 +3458,7 @@
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
       <c r="D136" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3358,7 +3466,7 @@
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
       <c r="D137" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3366,7 +3474,7 @@
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
       <c r="D138" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
     </row>
     <row r="139" spans="1:4">

</xml_diff>

<commit_message>
Add formatting of unoptimized reports and functinonality to merge unoptmized and optimized sections in each report
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Metrics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="131">
   <si>
     <t>Campaign Summary</t>
   </si>
@@ -426,8 +426,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -516,7 +517,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -600,8 +601,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -612,12 +619,16 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="30" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="29" applyFont="1"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="29" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="30" applyFont="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="29" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="89">
     <cellStyle name="Comma" xfId="29" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -659,6 +670,9 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -699,6 +713,9 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
@@ -1484,9 +1501,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C95"/>
+  <dimension ref="A2:C100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1514,56 +1531,78 @@
       <c r="A4" t="s">
         <v>54</v>
       </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>62</v>
       </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>63</v>
       </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
@@ -1582,84 +1621,98 @@
       <c r="A18" t="s">
         <v>41</v>
       </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>42</v>
       </c>
+      <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>44</v>
       </c>
+      <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>45</v>
       </c>
+      <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
+      <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>114</v>
       </c>
+      <c r="B24" s="7"/>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>66</v>
       </c>
+      <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>47</v>
       </c>
+      <c r="B26" s="7"/>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>111</v>
       </c>
+      <c r="B27" s="7"/>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>129</v>
       </c>
+      <c r="B28" s="7"/>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
+      <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>130</v>
       </c>
+      <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
+      <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1"/>
@@ -1683,39 +1736,46 @@
       <c r="A36" t="s">
         <v>69</v>
       </c>
+      <c r="B36" s="7"/>
       <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
+      <c r="B37" s="7"/>
       <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
+      <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>72</v>
       </c>
+      <c r="B39" s="7"/>
       <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>73</v>
       </c>
+      <c r="B40" s="7"/>
       <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>74</v>
       </c>
+      <c r="B41" s="7"/>
       <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:3">
+      <c r="B42" s="7"/>
       <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:3">
@@ -1735,90 +1795,105 @@
       <c r="A45" t="s">
         <v>2</v>
       </c>
+      <c r="B45" s="8"/>
       <c r="C45" s="8"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>41</v>
       </c>
+      <c r="B46" s="8"/>
       <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>42</v>
       </c>
+      <c r="B47" s="8"/>
       <c r="C47" s="8"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>43</v>
       </c>
+      <c r="B48" s="8"/>
       <c r="C48" s="8"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>44</v>
       </c>
+      <c r="B49" s="8"/>
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>45</v>
       </c>
+      <c r="B50" s="8"/>
       <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>46</v>
       </c>
+      <c r="B51" s="8"/>
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>114</v>
       </c>
+      <c r="B52" s="8"/>
       <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>66</v>
       </c>
+      <c r="B53" s="8"/>
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>47</v>
       </c>
+      <c r="B54" s="8"/>
       <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>111</v>
       </c>
+      <c r="B55" s="8"/>
       <c r="C55" s="8"/>
     </row>
     <row r="56" spans="1:3" s="5" customFormat="1">
       <c r="A56" s="6" t="s">
         <v>129</v>
       </c>
+      <c r="B56" s="9"/>
       <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="B57" s="8"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1">
       <c r="A58" s="6" t="s">
         <v>130</v>
       </c>
+      <c r="B58" s="9"/>
       <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1">
       <c r="A59" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="B59" s="9"/>
       <c r="C59" s="9"/>
     </row>
     <row r="61" spans="1:3">
@@ -1838,37 +1913,47 @@
       <c r="A63" t="s">
         <v>69</v>
       </c>
+      <c r="B63" s="8"/>
       <c r="C63" s="8"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
+      <c r="B64" s="8"/>
       <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>71</v>
       </c>
+      <c r="B65" s="8"/>
       <c r="C65" s="8"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>72</v>
       </c>
+      <c r="B66" s="8"/>
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>73</v>
       </c>
+      <c r="B67" s="8"/>
       <c r="C67" s="8"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>74</v>
       </c>
+      <c r="B68" s="8"/>
       <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
@@ -1887,91 +1972,110 @@
       <c r="A72" t="s">
         <v>2</v>
       </c>
+      <c r="B72" s="7"/>
       <c r="C72" s="7"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>41</v>
       </c>
+      <c r="B73" s="7"/>
       <c r="C73" s="7"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>42</v>
       </c>
+      <c r="B74" s="7"/>
       <c r="C74" s="7"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>43</v>
       </c>
+      <c r="B75" s="7"/>
       <c r="C75" s="7"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>44</v>
       </c>
+      <c r="B76" s="7"/>
       <c r="C76" s="7"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>45</v>
       </c>
+      <c r="B77" s="7"/>
       <c r="C77" s="7"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>46</v>
       </c>
+      <c r="B78" s="7"/>
       <c r="C78" s="7"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>114</v>
       </c>
+      <c r="B79" s="7"/>
       <c r="C79" s="7"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>66</v>
       </c>
+      <c r="B80" s="7"/>
       <c r="C80" s="7"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>47</v>
       </c>
+      <c r="B81" s="7"/>
       <c r="C81" s="7"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>111</v>
       </c>
+      <c r="B82" s="7"/>
       <c r="C82" s="7"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>129</v>
       </c>
+      <c r="B83" s="7"/>
       <c r="C83" s="7"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>48</v>
       </c>
+      <c r="B84" s="7"/>
       <c r="C84" s="7"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>130</v>
       </c>
+      <c r="B85" s="7"/>
       <c r="C85" s="7"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>49</v>
       </c>
+      <c r="B86" s="7"/>
       <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
@@ -1993,37 +2097,63 @@
       <c r="A90" t="s">
         <v>69</v>
       </c>
+      <c r="B90" s="7"/>
       <c r="C90" s="7"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>70</v>
       </c>
+      <c r="B91" s="7"/>
       <c r="C91" s="7"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>71</v>
       </c>
+      <c r="B92" s="7"/>
       <c r="C92" s="7"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>72</v>
       </c>
+      <c r="B93" s="7"/>
       <c r="C93" s="7"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>73</v>
       </c>
+      <c r="B94" s="7"/>
       <c r="C94" s="7"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>74</v>
       </c>
+      <c r="B95" s="7"/>
       <c r="C95" s="7"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+    </row>
+    <row r="97" spans="2:3">
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+    </row>
+    <row r="98" spans="2:3">
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+    </row>
+    <row r="99" spans="2:3">
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+    </row>
+    <row r="100" spans="2:3">
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2040,7 +2170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2066,73 +2196,194 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:17">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="J4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="N4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" s="1" customFormat="1">
-      <c r="A10" s="1" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:17" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
@@ -2197,143 +2448,143 @@
       <c r="A16" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-    </row>
-    <row r="22" spans="1:16" s="1" customFormat="1">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+    </row>
+    <row r="22" spans="1:17" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="1:17">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -2350,83 +2601,204 @@
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
     </row>
-    <row r="25" spans="1:16" s="1" customFormat="1">
+    <row r="25" spans="1:17" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1">
+    <row r="26" spans="1:17" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="1" customFormat="1">
-      <c r="B27" s="1" t="s">
+    <row r="27" spans="1:17">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="J27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="N27" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" s="13" customFormat="1">
       <c r="A28" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+    </row>
+    <row r="29" spans="1:17" s="13" customFormat="1">
       <c r="A29" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+    </row>
+    <row r="30" spans="1:17" s="13" customFormat="1">
       <c r="A30" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+    </row>
+    <row r="31" spans="1:17" s="13" customFormat="1">
       <c r="A31" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+    </row>
+    <row r="32" spans="1:17" s="13" customFormat="1">
       <c r="A32" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:17" s="1" customFormat="1">
-      <c r="A33" s="1" t="s">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+    </row>
+    <row r="33" spans="1:17" s="13" customFormat="1">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+    </row>
+    <row r="34" spans="1:17" s="14" customFormat="1">
+      <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
     </row>
     <row r="36" spans="1:17" s="1" customFormat="1">
       <c r="A36" s="1" t="s">
@@ -2611,21 +2983,21 @@
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
     </row>
     <row r="49" spans="1:17" s="1" customFormat="1">
       <c r="A49" s="1" t="s">
@@ -2638,72 +3010,193 @@
       </c>
     </row>
     <row r="51" spans="1:17">
-      <c r="B51" t="s">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C51" t="s">
+      <c r="J51" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M51" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D51" t="s">
+      <c r="N51" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O51" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E51" t="s">
+      <c r="P51" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="Q51" s="3"/>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
     </row>
     <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>86</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
     </row>
     <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:17" s="1" customFormat="1">
-      <c r="A57" s="1" t="s">
-        <v>82</v>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" t="s">
+        <v>89</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+    </row>
+    <row r="58" spans="1:17" s="1" customFormat="1">
+      <c r="A58" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1">
       <c r="A60" s="1" t="s">
@@ -2768,219 +3261,340 @@
       <c r="A63" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12"/>
-      <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12"/>
-      <c r="P63" s="12"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11"/>
+      <c r="O63" s="11"/>
+      <c r="P63" s="11"/>
     </row>
     <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
-      <c r="M64" s="12"/>
-      <c r="N64" s="12"/>
-      <c r="O64" s="12"/>
-      <c r="P64" s="12"/>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
-      <c r="M65" s="12"/>
-      <c r="N65" s="12"/>
-      <c r="O65" s="12"/>
-      <c r="P65" s="12"/>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="11"/>
+      <c r="P65" s="11"/>
+    </row>
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="12"/>
-      <c r="K66" s="12"/>
-      <c r="L66" s="12"/>
-      <c r="M66" s="12"/>
-      <c r="N66" s="12"/>
-      <c r="O66" s="12"/>
-      <c r="P66" s="12"/>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+    </row>
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>87</v>
       </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="12"/>
-      <c r="M67" s="12"/>
-      <c r="N67" s="12"/>
-      <c r="O67" s="12"/>
-      <c r="P67" s="12"/>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+      <c r="P67" s="11"/>
+    </row>
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>89</v>
       </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
-      <c r="M68" s="12"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="12"/>
-      <c r="P68" s="12"/>
-    </row>
-    <row r="69" spans="1:16" s="1" customFormat="1">
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="11"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="11"/>
+      <c r="O68" s="11"/>
+      <c r="P68" s="11"/>
+    </row>
+    <row r="69" spans="1:17" s="1" customFormat="1">
       <c r="A69" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13"/>
-      <c r="O69" s="13"/>
-      <c r="P69" s="13"/>
-    </row>
-    <row r="73" spans="1:16" s="1" customFormat="1">
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
+      <c r="P69" s="12"/>
+    </row>
+    <row r="73" spans="1:17" s="1" customFormat="1">
       <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1">
+    <row r="74" spans="1:17" s="1" customFormat="1">
       <c r="A74" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
-      <c r="B75" t="s">
+    <row r="75" spans="1:17">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I75" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C75" t="s">
+      <c r="J75" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M75" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D75" t="s">
+      <c r="N75" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O75" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E75" t="s">
+      <c r="P75" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="Q75" s="3"/>
+    </row>
+    <row r="76" spans="1:17" s="13" customFormat="1">
       <c r="A76" t="s">
         <v>83</v>
       </c>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-    </row>
-    <row r="77" spans="1:16">
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+    </row>
+    <row r="77" spans="1:17" s="13" customFormat="1">
       <c r="A77" t="s">
         <v>84</v>
       </c>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+    </row>
+    <row r="78" spans="1:17" s="13" customFormat="1">
       <c r="A78" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-    </row>
-    <row r="79" spans="1:16">
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+    </row>
+    <row r="79" spans="1:17" s="13" customFormat="1">
       <c r="A79" t="s">
         <v>86</v>
       </c>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
+    </row>
+    <row r="80" spans="1:17" s="13" customFormat="1">
       <c r="A80" t="s">
         <v>87</v>
       </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-    </row>
-    <row r="81" spans="1:17" s="1" customFormat="1">
-      <c r="A81" s="1" t="s">
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15"/>
+    </row>
+    <row r="81" spans="1:17" s="13" customFormat="1">
+      <c r="A81" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15"/>
+    </row>
+    <row r="82" spans="1:17" s="14" customFormat="1">
+      <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
+      <c r="L82" s="16"/>
+      <c r="M82" s="16"/>
+      <c r="N82" s="16"/>
+      <c r="O82" s="16"/>
+      <c r="P82" s="16"/>
     </row>
     <row r="85" spans="1:17" s="1" customFormat="1">
       <c r="A85" s="1" t="s">
@@ -3165,21 +3779,21 @@
       <c r="A94" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="11"/>
-      <c r="L94" s="11"/>
-      <c r="M94" s="11"/>
-      <c r="N94" s="11"/>
-      <c r="O94" s="11"/>
-      <c r="P94" s="11"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+      <c r="N94" s="10"/>
+      <c r="O94" s="10"/>
+      <c r="P94" s="10"/>
     </row>
     <row r="97" spans="1:3" s="1" customFormat="1">
       <c r="A97" s="1" t="s">

</xml_diff>

<commit_message>
Fix bugs reported by Lin - The total frequency and target frequency for the last two weeks in the Equivalized files are incorrect. - Some date and time format wasn’t loaded correctly. (format) - Alphabetical sorting: CNBC and Chiller are reversed. - Cell B4 (Total budget for Unoptimized Campaign) and C13 (Consumer Target Frequency for ATP Optimized campaign) (in Normalized 70 unequiv file it was B13 that has the issue) need correction.  C10 – can we make it two decimal points so it will be consistent with the rest?
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -517,7 +517,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -549,6 +549,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -628,7 +636,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="97">
     <cellStyle name="Comma" xfId="29" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -673,6 +681,10 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -716,6 +728,10 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
@@ -1452,10 +1468,10 @@
         <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>44</v>
@@ -1573,8 +1589,8 @@
       <c r="A10" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -1626,14 +1642,14 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1807,14 +1823,14 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -1984,14 +2000,14 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2202,10 +2218,10 @@
         <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>44</v>
@@ -2401,10 +2417,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>44</v>
@@ -2617,10 +2633,10 @@
         <v>41</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>44</v>
@@ -2816,10 +2832,10 @@
         <v>41</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>44</v>
@@ -3015,10 +3031,10 @@
         <v>41</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>44</v>
@@ -3214,10 +3230,10 @@
         <v>41</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>44</v>
@@ -3413,10 +3429,10 @@
         <v>41</v>
       </c>
       <c r="C75" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>44</v>
@@ -3612,10 +3628,10 @@
         <v>41</v>
       </c>
       <c r="C87" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>44</v>
@@ -3824,14 +3840,14 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -4000,7 +4016,7 @@
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
       <c r="D127" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -4008,7 +4024,7 @@
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
       <c r="D128" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="129" spans="1:4">

</xml_diff>

<commit_message>
Add 'NBC Universo' to reports 1
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="3620" yWindow="-20720" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Metrics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="134">
   <si>
     <t>Campaign Summary</t>
   </si>
@@ -420,6 +420,15 @@
   </si>
   <si>
     <t>Telemundo</t>
+  </si>
+  <si>
+    <t>Total (NBC Universo)</t>
+  </si>
+  <si>
+    <t>Target (NBC Universo)</t>
+  </si>
+  <si>
+    <t>NBC Universo</t>
   </si>
 </sst>
 </file>
@@ -430,7 +439,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -499,6 +508,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -517,7 +533,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -615,8 +631,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -635,8 +661,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="107">
     <cellStyle name="Comma" xfId="29" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -685,6 +712,11 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -732,6 +764,11 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
@@ -1320,19 +1357,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AC3"/>
+  <dimension ref="A3:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="25" width="19.6640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="19.6640625" style="1" customWidth="1"/>
+    <col min="1" max="18" width="19.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5" style="1" customWidth="1"/>
+    <col min="20" max="27" width="19.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="19.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:31">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1385,39 +1424,45 @@
         <v>35</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1434,7 +1479,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:R3"/>
+  <dimension ref="A3:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1444,14 +1489,14 @@
     <col min="2" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="14" width="25.6640625" customWidth="1"/>
-    <col min="15" max="15" width="25.1640625" customWidth="1"/>
-    <col min="16" max="16" width="25.6640625" customWidth="1"/>
-    <col min="17" max="17" width="25.1640625" customWidth="1"/>
-    <col min="18" max="18" width="25.6640625" customWidth="1"/>
+    <col min="6" max="15" width="25.6640625" customWidth="1"/>
+    <col min="16" max="16" width="25.1640625" customWidth="1"/>
+    <col min="17" max="17" width="25.6640625" customWidth="1"/>
+    <col min="18" max="18" width="25.1640625" customWidth="1"/>
+    <col min="19" max="19" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" s="1" customFormat="1">
+    <row r="3" spans="1:19" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -1486,21 +1531,24 @@
         <v>114</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1517,7 +1565,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C100"/>
+  <dimension ref="A2:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1691,485 +1739,506 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>48</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" s="5" customFormat="1"/>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" s="5" customFormat="1"/>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="B35" t="s">
+    <row r="36" spans="1:3">
+      <c r="B36" t="s">
         <v>52</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>74</v>
+      </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="B44" t="s">
+    <row r="45" spans="1:3">
+      <c r="B45" t="s">
         <v>52</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>111</v>
+      <c r="A55" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:3" s="5" customFormat="1">
-      <c r="A56" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="6" t="s">
-        <v>48</v>
+      <c r="A57" t="s">
+        <v>111</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1">
       <c r="A58" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
     </row>
-    <row r="59" spans="1:3" s="5" customFormat="1">
+    <row r="59" spans="1:3">
       <c r="A59" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:3" s="5" customFormat="1">
+      <c r="A60" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+    </row>
+    <row r="61" spans="1:3" s="5" customFormat="1">
+      <c r="A61" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="B62" t="s">
+    <row r="64" spans="1:3">
+      <c r="B64" t="s">
         <v>52</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>69</v>
-      </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="B71" t="s">
+    <row r="73" spans="1:3">
+      <c r="B73" t="s">
         <v>52</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>41</v>
-      </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>114</v>
+        <v>45</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
     </row>
     <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>48</v>
+      </c>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="A88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>79</v>
-      </c>
-      <c r="B89" t="s">
-        <v>52</v>
-      </c>
-      <c r="C89" t="s">
-        <v>53</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" t="s">
-        <v>69</v>
-      </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>70</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
+      <c r="A91" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>71</v>
-      </c>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B92" t="s">
+        <v>52</v>
+      </c>
+      <c r="C92" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
     </row>
     <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>72</v>
+      </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
     </row>
-    <row r="97" spans="2:3">
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>73</v>
+      </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>74</v>
+      </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
     </row>
-    <row r="99" spans="2:3">
+    <row r="99" spans="1:3">
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
     </row>
-    <row r="100" spans="2:3">
+    <row r="100" spans="1:3">
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2184,7 +2253,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q145"/>
+  <dimension ref="A1:R147"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2194,25 +2263,25 @@
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="15" width="14.5" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" customWidth="1"/>
-    <col min="17" max="20" width="37" customWidth="1"/>
+    <col min="5" max="16" width="14.5" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" customWidth="1"/>
+    <col min="18" max="21" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>41</v>
@@ -2239,29 +2308,32 @@
         <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -2280,8 +2352,9 @@
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -2300,8 +2373,9 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -2320,8 +2394,9 @@
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2340,8 +2415,9 @@
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -2360,8 +2436,9 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2380,8 +2457,9 @@
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
-    </row>
-    <row r="11" spans="1:17" s="1" customFormat="1">
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:18" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
@@ -2400,18 +2478,19 @@
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="Q11" s="12"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>41</v>
@@ -2438,29 +2517,32 @@
         <v>66</v>
       </c>
       <c r="J15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="O15" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -2479,8 +2561,9 @@
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="Q16" s="11"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -2499,8 +2582,9 @@
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="Q17" s="11"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -2519,8 +2603,9 @@
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="Q18" s="11"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -2539,8 +2624,9 @@
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="Q19" s="11"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -2559,8 +2645,9 @@
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
       <c r="P20" s="11"/>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="Q20" s="11"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -2579,8 +2666,9 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
-    </row>
-    <row r="22" spans="1:17" s="1" customFormat="1">
+      <c r="Q21" s="11"/>
+    </row>
+    <row r="22" spans="1:18" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
@@ -2599,8 +2687,9 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="Q22" s="12"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -2616,18 +2705,19 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
-    </row>
-    <row r="25" spans="1:17" s="1" customFormat="1">
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="25" spans="1:18" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="1" customFormat="1">
+    <row r="26" spans="1:18" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:18">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>41</v>
@@ -2654,29 +2744,32 @@
         <v>66</v>
       </c>
       <c r="J27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="N27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N27" s="3" t="s">
+      <c r="O27" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="P27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q27" s="3"/>
-    </row>
-    <row r="28" spans="1:17" s="13" customFormat="1">
+      <c r="R27" s="3"/>
+    </row>
+    <row r="28" spans="1:18" s="13" customFormat="1">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2695,8 +2788,9 @@
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
-    </row>
-    <row r="29" spans="1:17" s="13" customFormat="1">
+      <c r="Q28" s="15"/>
+    </row>
+    <row r="29" spans="1:18" s="13" customFormat="1">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -2715,8 +2809,9 @@
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
-    </row>
-    <row r="30" spans="1:17" s="13" customFormat="1">
+      <c r="Q29" s="15"/>
+    </row>
+    <row r="30" spans="1:18" s="13" customFormat="1">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2735,8 +2830,9 @@
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
-    </row>
-    <row r="31" spans="1:17" s="13" customFormat="1">
+      <c r="Q30" s="15"/>
+    </row>
+    <row r="31" spans="1:18" s="13" customFormat="1">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -2755,8 +2851,9 @@
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
-    </row>
-    <row r="32" spans="1:17" s="13" customFormat="1">
+      <c r="Q31" s="15"/>
+    </row>
+    <row r="32" spans="1:18" s="13" customFormat="1">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -2775,8 +2872,9 @@
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
       <c r="P32" s="15"/>
-    </row>
-    <row r="33" spans="1:17" s="13" customFormat="1">
+      <c r="Q32" s="15"/>
+    </row>
+    <row r="33" spans="1:18" s="13" customFormat="1">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2795,8 +2893,9 @@
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
-    </row>
-    <row r="34" spans="1:17" s="14" customFormat="1">
+      <c r="Q33" s="15"/>
+    </row>
+    <row r="34" spans="1:18" s="14" customFormat="1">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
@@ -2815,18 +2914,19 @@
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
       <c r="P34" s="16"/>
-    </row>
-    <row r="36" spans="1:17" s="1" customFormat="1">
+      <c r="Q34" s="16"/>
+    </row>
+    <row r="36" spans="1:18" s="1" customFormat="1">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1">
+    <row r="37" spans="1:18" s="1" customFormat="1">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:18">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>41</v>
@@ -2853,29 +2953,32 @@
         <v>66</v>
       </c>
       <c r="J38" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M38" s="3" t="s">
+      <c r="N38" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N38" s="3" t="s">
+      <c r="O38" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O38" s="3" t="s">
+      <c r="P38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q38" s="3"/>
-    </row>
-    <row r="39" spans="1:17">
+      <c r="R38" s="3"/>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -2894,8 +2997,9 @@
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="Q39" s="8"/>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -2914,8 +3018,9 @@
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
       <c r="P40" s="8"/>
-    </row>
-    <row r="41" spans="1:17">
+      <c r="Q40" s="8"/>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2934,8 +3039,9 @@
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="Q41" s="8"/>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -2954,8 +3060,9 @@
       <c r="N42" s="8"/>
       <c r="O42" s="8"/>
       <c r="P42" s="8"/>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="Q42" s="8"/>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -2974,8 +3081,9 @@
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
       <c r="P43" s="8"/>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="Q43" s="8"/>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2994,8 +3102,9 @@
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
       <c r="P44" s="8"/>
-    </row>
-    <row r="45" spans="1:17" s="1" customFormat="1">
+      <c r="Q44" s="8"/>
+    </row>
+    <row r="45" spans="1:18" s="1" customFormat="1">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
@@ -3014,18 +3123,19 @@
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
-    </row>
-    <row r="49" spans="1:17" s="1" customFormat="1">
+      <c r="Q45" s="10"/>
+    </row>
+    <row r="49" spans="1:18" s="1" customFormat="1">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="1" customFormat="1">
+    <row r="50" spans="1:18" s="1" customFormat="1">
       <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:18">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
         <v>41</v>
@@ -3052,29 +3162,32 @@
         <v>66</v>
       </c>
       <c r="J51" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K51" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L51" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M51" s="3" t="s">
+      <c r="N51" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N51" s="3" t="s">
+      <c r="O51" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O51" s="3" t="s">
+      <c r="P51" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P51" s="1" t="s">
+      <c r="Q51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q51" s="3"/>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="R51" s="3"/>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -3093,8 +3206,9 @@
       <c r="N52" s="11"/>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
-    </row>
-    <row r="53" spans="1:17">
+      <c r="Q52" s="11"/>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53" t="s">
         <v>84</v>
       </c>
@@ -3113,8 +3227,9 @@
       <c r="N53" s="11"/>
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="Q53" s="11"/>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -3133,8 +3248,9 @@
       <c r="N54" s="11"/>
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
-    </row>
-    <row r="55" spans="1:17">
+      <c r="Q54" s="11"/>
+    </row>
+    <row r="55" spans="1:18">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -3153,8 +3269,9 @@
       <c r="N55" s="11"/>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
-    </row>
-    <row r="56" spans="1:17">
+      <c r="Q55" s="11"/>
+    </row>
+    <row r="56" spans="1:18">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -3173,8 +3290,9 @@
       <c r="N56" s="11"/>
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
-    </row>
-    <row r="57" spans="1:17">
+      <c r="Q56" s="11"/>
+    </row>
+    <row r="57" spans="1:18">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -3193,8 +3311,9 @@
       <c r="N57" s="11"/>
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
-    </row>
-    <row r="58" spans="1:17" s="1" customFormat="1">
+      <c r="Q57" s="11"/>
+    </row>
+    <row r="58" spans="1:18" s="1" customFormat="1">
       <c r="A58" s="1" t="s">
         <v>82</v>
       </c>
@@ -3213,18 +3332,19 @@
       <c r="N58" s="12"/>
       <c r="O58" s="12"/>
       <c r="P58" s="12"/>
-    </row>
-    <row r="60" spans="1:17" s="1" customFormat="1">
+      <c r="Q58" s="12"/>
+    </row>
+    <row r="60" spans="1:18" s="1" customFormat="1">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="1" customFormat="1">
+    <row r="61" spans="1:18" s="1" customFormat="1">
       <c r="A61" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:18">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
         <v>41</v>
@@ -3251,29 +3371,32 @@
         <v>66</v>
       </c>
       <c r="J62" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K62" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="L62" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L62" s="1" t="s">
+      <c r="M62" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M62" s="3" t="s">
+      <c r="N62" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N62" s="3" t="s">
+      <c r="O62" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O62" s="3" t="s">
+      <c r="P62" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P62" s="1" t="s">
+      <c r="Q62" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q62" s="3"/>
-    </row>
-    <row r="63" spans="1:17">
+      <c r="R62" s="3"/>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63" t="s">
         <v>83</v>
       </c>
@@ -3292,8 +3415,9 @@
       <c r="N63" s="11"/>
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
-    </row>
-    <row r="64" spans="1:17">
+      <c r="Q63" s="11"/>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -3312,8 +3436,9 @@
       <c r="N64" s="11"/>
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
-    </row>
-    <row r="65" spans="1:17">
+      <c r="Q64" s="11"/>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -3332,8 +3457,9 @@
       <c r="N65" s="11"/>
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
-    </row>
-    <row r="66" spans="1:17">
+      <c r="Q65" s="11"/>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -3352,8 +3478,9 @@
       <c r="N66" s="11"/>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
-    </row>
-    <row r="67" spans="1:17">
+      <c r="Q66" s="11"/>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67" t="s">
         <v>87</v>
       </c>
@@ -3372,8 +3499,9 @@
       <c r="N67" s="11"/>
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
-    </row>
-    <row r="68" spans="1:17">
+      <c r="Q67" s="11"/>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68" t="s">
         <v>89</v>
       </c>
@@ -3392,8 +3520,9 @@
       <c r="N68" s="11"/>
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
-    </row>
-    <row r="69" spans="1:17" s="1" customFormat="1">
+      <c r="Q68" s="11"/>
+    </row>
+    <row r="69" spans="1:18" s="1" customFormat="1">
       <c r="A69" s="1" t="s">
         <v>82</v>
       </c>
@@ -3412,18 +3541,19 @@
       <c r="N69" s="12"/>
       <c r="O69" s="12"/>
       <c r="P69" s="12"/>
-    </row>
-    <row r="73" spans="1:17" s="1" customFormat="1">
+      <c r="Q69" s="12"/>
+    </row>
+    <row r="73" spans="1:18" s="1" customFormat="1">
       <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:17" s="1" customFormat="1">
+    <row r="74" spans="1:18" s="1" customFormat="1">
       <c r="A74" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:18">
       <c r="A75" s="3"/>
       <c r="B75" s="3" t="s">
         <v>41</v>
@@ -3450,29 +3580,32 @@
         <v>66</v>
       </c>
       <c r="J75" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K75" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="L75" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L75" s="1" t="s">
+      <c r="M75" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M75" s="3" t="s">
+      <c r="N75" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N75" s="3" t="s">
+      <c r="O75" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O75" s="3" t="s">
+      <c r="P75" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P75" s="1" t="s">
+      <c r="Q75" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q75" s="3"/>
-    </row>
-    <row r="76" spans="1:17" s="13" customFormat="1">
+      <c r="R75" s="3"/>
+    </row>
+    <row r="76" spans="1:18" s="13" customFormat="1">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -3491,8 +3624,9 @@
       <c r="N76" s="15"/>
       <c r="O76" s="15"/>
       <c r="P76" s="15"/>
-    </row>
-    <row r="77" spans="1:17" s="13" customFormat="1">
+      <c r="Q76" s="15"/>
+    </row>
+    <row r="77" spans="1:18" s="13" customFormat="1">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -3511,8 +3645,9 @@
       <c r="N77" s="15"/>
       <c r="O77" s="15"/>
       <c r="P77" s="15"/>
-    </row>
-    <row r="78" spans="1:17" s="13" customFormat="1">
+      <c r="Q77" s="15"/>
+    </row>
+    <row r="78" spans="1:18" s="13" customFormat="1">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -3531,8 +3666,9 @@
       <c r="N78" s="15"/>
       <c r="O78" s="15"/>
       <c r="P78" s="15"/>
-    </row>
-    <row r="79" spans="1:17" s="13" customFormat="1">
+      <c r="Q78" s="15"/>
+    </row>
+    <row r="79" spans="1:18" s="13" customFormat="1">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -3551,8 +3687,9 @@
       <c r="N79" s="15"/>
       <c r="O79" s="15"/>
       <c r="P79" s="15"/>
-    </row>
-    <row r="80" spans="1:17" s="13" customFormat="1">
+      <c r="Q79" s="15"/>
+    </row>
+    <row r="80" spans="1:18" s="13" customFormat="1">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -3571,8 +3708,9 @@
       <c r="N80" s="15"/>
       <c r="O80" s="15"/>
       <c r="P80" s="15"/>
-    </row>
-    <row r="81" spans="1:17" s="13" customFormat="1">
+      <c r="Q80" s="15"/>
+    </row>
+    <row r="81" spans="1:18" s="13" customFormat="1">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -3591,8 +3729,9 @@
       <c r="N81" s="15"/>
       <c r="O81" s="15"/>
       <c r="P81" s="15"/>
-    </row>
-    <row r="82" spans="1:17" s="14" customFormat="1">
+      <c r="Q81" s="15"/>
+    </row>
+    <row r="82" spans="1:18" s="14" customFormat="1">
       <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
@@ -3611,18 +3750,19 @@
       <c r="N82" s="16"/>
       <c r="O82" s="16"/>
       <c r="P82" s="16"/>
-    </row>
-    <row r="85" spans="1:17" s="1" customFormat="1">
+      <c r="Q82" s="16"/>
+    </row>
+    <row r="85" spans="1:18" s="1" customFormat="1">
       <c r="A85" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:17" s="1" customFormat="1">
+    <row r="86" spans="1:18" s="1" customFormat="1">
       <c r="A86" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:18">
       <c r="A87" s="3"/>
       <c r="B87" s="3" t="s">
         <v>41</v>
@@ -3649,29 +3789,32 @@
         <v>66</v>
       </c>
       <c r="J87" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K87" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K87" s="1" t="s">
+      <c r="L87" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="L87" s="1" t="s">
+      <c r="M87" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M87" s="3" t="s">
+      <c r="N87" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N87" s="3" t="s">
+      <c r="O87" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O87" s="3" t="s">
+      <c r="P87" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P87" s="1" t="s">
+      <c r="Q87" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q87" s="3"/>
-    </row>
-    <row r="88" spans="1:17">
+      <c r="R87" s="3"/>
+    </row>
+    <row r="88" spans="1:18">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -3690,8 +3833,9 @@
       <c r="N88" s="8"/>
       <c r="O88" s="8"/>
       <c r="P88" s="8"/>
-    </row>
-    <row r="89" spans="1:17">
+      <c r="Q88" s="8"/>
+    </row>
+    <row r="89" spans="1:18">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -3710,8 +3854,9 @@
       <c r="N89" s="8"/>
       <c r="O89" s="8"/>
       <c r="P89" s="8"/>
-    </row>
-    <row r="90" spans="1:17">
+      <c r="Q89" s="8"/>
+    </row>
+    <row r="90" spans="1:18">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -3730,8 +3875,9 @@
       <c r="N90" s="8"/>
       <c r="O90" s="8"/>
       <c r="P90" s="8"/>
-    </row>
-    <row r="91" spans="1:17">
+      <c r="Q90" s="8"/>
+    </row>
+    <row r="91" spans="1:18">
       <c r="A91" t="s">
         <v>86</v>
       </c>
@@ -3750,8 +3896,9 @@
       <c r="N91" s="8"/>
       <c r="O91" s="8"/>
       <c r="P91" s="8"/>
-    </row>
-    <row r="92" spans="1:17">
+      <c r="Q91" s="8"/>
+    </row>
+    <row r="92" spans="1:18">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -3770,8 +3917,9 @@
       <c r="N92" s="8"/>
       <c r="O92" s="8"/>
       <c r="P92" s="8"/>
-    </row>
-    <row r="93" spans="1:17">
+      <c r="Q92" s="8"/>
+    </row>
+    <row r="93" spans="1:18">
       <c r="A93" t="s">
         <v>89</v>
       </c>
@@ -3790,8 +3938,9 @@
       <c r="N93" s="8"/>
       <c r="O93" s="8"/>
       <c r="P93" s="8"/>
-    </row>
-    <row r="94" spans="1:17" s="1" customFormat="1">
+      <c r="Q93" s="8"/>
+    </row>
+    <row r="94" spans="1:18" s="1" customFormat="1">
       <c r="A94" s="1" t="s">
         <v>82</v>
       </c>
@@ -3810,6 +3959,7 @@
       <c r="N94" s="10"/>
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
+      <c r="Q94" s="10"/>
     </row>
     <row r="97" spans="1:3" s="1" customFormat="1">
       <c r="A97" s="1" t="s">
@@ -3889,126 +4039,125 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>130</v>
+        <v>48</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
     </row>
-    <row r="115" spans="1:4" s="1" customFormat="1">
-      <c r="A115" s="1" t="s">
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>49</v>
+      </c>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+    </row>
+    <row r="116" spans="1:4" s="1" customFormat="1">
+      <c r="A116" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
-      <c r="B116" t="s">
+    <row r="117" spans="1:4">
+      <c r="B117" t="s">
         <v>52</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" t="s">
-        <v>83</v>
-      </c>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
     </row>
-    <row r="124" spans="1:4" s="1" customFormat="1">
-      <c r="A124" s="1" t="s">
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>89</v>
+      </c>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+    </row>
+    <row r="125" spans="1:4" s="1" customFormat="1">
+      <c r="A125" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
-      <c r="A125" t="s">
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
         <v>104</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>105</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>106</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D126" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" s="8"/>
-      <c r="B126" s="8"/>
-      <c r="C126" s="8"/>
-      <c r="D126" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -4016,7 +4165,7 @@
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
       <c r="D127" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -4024,7 +4173,7 @@
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
       <c r="D128" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -4032,7 +4181,7 @@
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
       <c r="D129" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -4040,7 +4189,7 @@
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
       <c r="D130" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -4048,7 +4197,7 @@
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
       <c r="D131" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -4056,7 +4205,7 @@
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
       <c r="D132" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -4064,7 +4213,7 @@
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
       <c r="D133" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -4072,7 +4221,7 @@
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
       <c r="D134" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -4080,7 +4229,7 @@
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
       <c r="D135" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -4088,7 +4237,7 @@
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
       <c r="D136" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -4096,7 +4245,7 @@
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
       <c r="D137" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -4104,7 +4253,7 @@
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
       <c r="D138" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -4112,7 +4261,7 @@
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
       <c r="D139" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -4120,7 +4269,7 @@
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
       <c r="D140" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -4128,7 +4277,7 @@
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
       <c r="D141" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -4136,7 +4285,7 @@
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
       <c r="D142" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -4144,7 +4293,7 @@
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
       <c r="D143" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -4152,11 +4301,27 @@
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
       <c r="D144" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="8"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="8"/>
+      <c r="D145" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="8"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
-      <c r="A145" s="2" t="s">
+    <row r="147" spans="1:4">
+      <c r="A147" s="2" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>